<commit_message>
Customize MOfEDS for heavy fuel oil plants
</commit_message>
<xml_diff>
--- a/InputData/elec/MOfEDS/Manual Override for Elec Dispatch Shareweights.xlsx
+++ b/InputData/elec/MOfEDS/Manual Override for Elec Dispatch Shareweights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\elec\MOfEDS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-mexico\InputData\elec\MOfEDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC387BE5-DC79-427F-B7DB-D3B25D54F9CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34DCB3AC-3261-492F-9BBB-6FD56CB93334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="21315" yWindow="915" windowWidth="27495" windowHeight="19425" xr2:uid="{5214CE78-272C-4AF8-83F6-52B9106E2D78}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{5214CE78-272C-4AF8-83F6-52B9106E2D78}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -566,14 +566,14 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -581,32 +581,32 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
@@ -620,27 +620,27 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>13</v>
       </c>
@@ -654,42 +654,42 @@
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -704,14 +704,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E636F4FF-3519-4D1A-B2AD-0AD071209429}">
   <dimension ref="A1:AF17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B1">
         <v>2020</v>
       </c>
@@ -806,7 +808,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -904,7 +906,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -1002,7 +1004,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -1100,7 +1102,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -1198,7 +1200,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -1296,7 +1298,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -1394,7 +1396,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -1492,7 +1494,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -1590,7 +1592,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -1688,7 +1690,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -1786,7 +1788,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -1884,7 +1886,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -1982,7 +1984,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -2080,7 +2082,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -2178,105 +2180,105 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>36</v>
       </c>
       <c r="B16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="C16">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="E16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="F16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="G16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="H16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="I16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="J16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="K16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="L16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="M16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="N16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="O16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="P16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="Q16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="R16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="S16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="T16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="U16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="V16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="W16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="X16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="Y16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="Z16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="AA16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="AB16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="AC16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="AD16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="AE16">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="AF16">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -2385,12 +2387,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B1">
         <v>2020</v>
       </c>
@@ -2485,7 +2487,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -2583,7 +2585,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -2681,7 +2683,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -2779,7 +2781,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -2877,7 +2879,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -2975,7 +2977,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -3073,7 +3075,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -3171,7 +3173,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -3269,7 +3271,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -3367,7 +3369,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -3465,7 +3467,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -3563,7 +3565,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -3661,7 +3663,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -3759,7 +3761,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -3857,7 +3859,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -3955,7 +3957,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>37</v>
       </c>
@@ -4064,12 +4066,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="24.7109375" customWidth="1"/>
+    <col min="1" max="1" width="24.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.35">
       <c r="B1">
         <v>2020</v>
       </c>
@@ -4164,7 +4166,7 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -4262,7 +4264,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>23</v>
       </c>
@@ -4360,7 +4362,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>24</v>
       </c>
@@ -4458,7 +4460,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>25</v>
       </c>
@@ -4556,7 +4558,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>26</v>
       </c>
@@ -4654,7 +4656,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>27</v>
       </c>
@@ -4752,7 +4754,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -4850,7 +4852,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>29</v>
       </c>
@@ -4948,7 +4950,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>30</v>
       </c>
@@ -5046,7 +5048,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>31</v>
       </c>
@@ -5144,7 +5146,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>32</v>
       </c>
@@ -5242,7 +5244,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>33</v>
       </c>
@@ -5340,7 +5342,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>34</v>
       </c>
@@ -5438,7 +5440,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>35</v>
       </c>
@@ -5536,7 +5538,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -5634,7 +5636,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>37</v>
       </c>

</xml_diff>